<commit_message>
deleted:    Catapult/README.md 	deleted:    Catapult/catapult_config.json 	renamed:    Catapult/Catapult_cpp_1_0.cpp -> Enter/Catapult/Catapult_cpp_1_0.cpp 	new file:   Enter/Catapult/README.md 	modified:   Enter/enter_config.json 	modified:   Enter/enter_test_info.xlsx 	modified:   Enter/read_info.py 	modified:   Jack/README.md 	modified:   Jack/batch_test/Jack_cpp_1_0.cpp 	deleted:    Jack/batch_test/jack_config.json 	deleted:    Jack/batch_test/jack_test_info.xlsx 	deleted:    Jack/batch_test/read_info.py 	modified:   Jack/jack_config.json 	modified:   Jack/jack_test_info.xlsx 	modified:   Jack/read_info.py 	modified:   Zomboni/README.md 	modified:   Zomboni/Zomboni_cpp_1_0.cpp 	modified:   Zomboni/zomboni_config.json 	modified:   Zomboni/zomboni_test_info.xlsx 	modified:   inc/calculate_position.hpp 	modified:   inc/common.hpp 	modified:   inc/tools/Enter.hpp 	modified:   inc/tools/Jack.hpp
</commit_message>
<xml_diff>
--- a/Zomboni/zomboni_test_info.xlsx
+++ b/Zomboni/zomboni_test_info.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="32460" windowHeight="16660" firstSheet="2"/>
+    <workbookView windowWidth="27750" windowHeight="10665"/>
   </bookViews>
   <sheets>
-    <sheet name="守六" sheetId="1" r:id="rId1"/>
-    <sheet name="守八" sheetId="2" r:id="rId2"/>
-    <sheet name="守五" sheetId="8" r:id="rId3"/>
-    <sheet name="tmp" sheetId="4" r:id="rId4"/>
-    <sheet name="守七" sheetId="7" r:id="rId5"/>
-    <sheet name="守四" sheetId="6" r:id="rId6"/>
+    <sheet name="守一" sheetId="9" r:id="rId1"/>
+    <sheet name="守五" sheetId="8" r:id="rId2"/>
+    <sheet name="tmp" sheetId="4" r:id="rId3"/>
+    <sheet name="守六" sheetId="1" r:id="rId4"/>
+    <sheet name="守八" sheetId="2" r:id="rId5"/>
+    <sheet name="守七" sheetId="7" r:id="rId6"/>
+    <sheet name="守四" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="22">
   <si>
     <t>被压列数</t>
   </si>
@@ -79,28 +80,25 @@
     <t>测试次数</t>
   </si>
   <si>
+    <t>非永动</t>
+  </si>
+  <si>
     <t>是否展示测试进度</t>
   </si>
   <si>
     <t>是</t>
   </si>
   <si>
-    <t>锁植物反应</t>
+    <t>锁植物攻击间隔</t>
   </si>
   <si>
-    <t>最慢</t>
-  </si>
-  <si>
-    <t>非永动</t>
+    <t>随机</t>
   </si>
   <si>
     <t>时间上限</t>
   </si>
   <si>
     <t>喷</t>
-  </si>
-  <si>
-    <t>随机</t>
   </si>
 </sst>
 </file>
@@ -287,6 +285,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -365,12 +375,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -408,12 +412,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -604,7 +602,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -628,16 +626,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -646,60 +644,60 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -728,7 +726,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -748,6 +746,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1274,34 +1278,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
+  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="17.3653846153846" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.69230769230769" style="1"/>
-    <col min="3" max="3" width="9.23076923076923" style="1"/>
-    <col min="4" max="7" width="9.23076923076923" style="2"/>
-    <col min="8" max="8" width="9.23076923076923" style="1"/>
-    <col min="9" max="9" width="10.0096153846154" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9.23076923076923" style="2"/>
-    <col min="12" max="12" width="9.23076923076923" style="1"/>
-    <col min="13" max="13" width="10.8653846153846" style="2" customWidth="1"/>
-    <col min="14" max="15" width="9.23076923076923" style="2"/>
-    <col min="16" max="16384" width="9.23076923076923" style="1"/>
+    <col min="1" max="1" width="17.3666666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.69166666666667" style="1"/>
+    <col min="3" max="3" width="9.23333333333333" style="1"/>
+    <col min="4" max="7" width="9.23333333333333" style="2"/>
+    <col min="8" max="8" width="9.23333333333333" style="1"/>
+    <col min="9" max="9" width="10.0083333333333" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9.23333333333333" style="2"/>
+    <col min="12" max="12" width="9.23333333333333" style="1"/>
+    <col min="13" max="13" width="10.8666666666667" style="2" customWidth="1"/>
+    <col min="14" max="15" width="9.23333333333333" style="2"/>
+    <col min="16" max="16384" width="9.23333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" s="1" customFormat="1" spans="1:15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -1320,7 +1324,7 @@
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" s="1" customFormat="1" spans="1:15">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1358,7 +1362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="4:15">
+    <row r="3" s="1" customFormat="1" spans="1:15">
       <c r="D3" s="6">
         <v>7</v>
       </c>
@@ -1378,13 +1382,13 @@
         <v>13</v>
       </c>
       <c r="K3" s="6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" s="1" customFormat="1" spans="1:15">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -1392,16 +1396,16 @@
         <v>1000000</v>
       </c>
       <c r="D4" s="6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G4" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4" s="4">
         <v>0.5</v>
@@ -1410,30 +1414,30 @@
         <v>13</v>
       </c>
       <c r="K4" s="6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" s="1" customFormat="1" spans="1:15">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G5" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I5" s="4">
         <v>0.25</v>
@@ -1448,12 +1452,12 @@
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
     </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="4" t="s">
+    <row r="6" s="1" customFormat="1" spans="1:15">
+      <c r="A6" s="7" t="s">
         <v>18</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="D6" s="6">
         <v>5</v>
@@ -1462,7 +1466,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
@@ -1480,7 +1484,7 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" s="1" customFormat="1" spans="1:15">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -1512,7 +1516,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" spans="4:15">
+    <row r="8" s="1" customFormat="1" spans="1:15">
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -1530,7 +1534,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" spans="4:15">
+    <row r="9" s="1" customFormat="1" spans="1:15">
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -1542,7 +1546,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="4:15">
+    <row r="10" s="1" customFormat="1" spans="1:15">
       <c r="D10" s="6">
         <v>6</v>
       </c>
@@ -1568,7 +1572,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="4:15">
+    <row r="11" s="1" customFormat="1" spans="1:15">
       <c r="D11" s="6">
         <v>5</v>
       </c>
@@ -1579,7 +1583,7 @@
         <v>13</v>
       </c>
       <c r="G11" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" s="4">
         <v>1.375</v>
@@ -1594,7 +1598,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="4:15">
+    <row r="12" s="1" customFormat="1" spans="1:15">
       <c r="D12" s="6">
         <v>4</v>
       </c>
@@ -1605,7 +1609,7 @@
         <v>13</v>
       </c>
       <c r="G12" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" s="4">
         <v>1.375</v>
@@ -1620,7 +1624,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="4:15">
+    <row r="13" s="1" customFormat="1" spans="1:15">
       <c r="D13" s="6">
         <v>3</v>
       </c>
@@ -1646,7 +1650,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="4:15">
+    <row r="14" s="1" customFormat="1" spans="1:15">
       <c r="D14" s="6">
         <v>2</v>
       </c>
@@ -1672,7 +1676,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="4:15">
+    <row r="15" s="1" customFormat="1" spans="1:15">
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -1690,7 +1694,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="4:15">
+    <row r="16" s="1" customFormat="1" spans="1:15">
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -1702,7 +1706,7 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" spans="4:15">
+    <row r="17" s="1" customFormat="1" spans="4:15">
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -1720,7 +1724,7 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" spans="4:15">
+    <row r="18" s="1" customFormat="1" spans="4:15">
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -1739,7 +1743,7 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
     </row>
-    <row r="19" spans="4:15">
+    <row r="19" s="1" customFormat="1" spans="4:15">
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -1751,7 +1755,7 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
     </row>
-    <row r="20" spans="4:15">
+    <row r="20" s="1" customFormat="1" spans="4:15">
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -1763,7 +1767,7 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
     </row>
-    <row r="21" spans="4:15">
+    <row r="21" s="1" customFormat="1" spans="4:15">
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -1775,7 +1779,7 @@
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
     </row>
-    <row r="22" spans="4:15">
+    <row r="22" s="1" customFormat="1" spans="4:15">
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -1787,7 +1791,7 @@
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
     </row>
-    <row r="23" spans="4:15">
+    <row r="23" s="1" customFormat="1" spans="4:15">
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -1799,7 +1803,7 @@
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
     </row>
-    <row r="24" spans="4:15">
+    <row r="24" s="1" customFormat="1" spans="4:15">
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -1811,7 +1815,7 @@
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
     </row>
-    <row r="25" spans="4:15">
+    <row r="25" s="1" customFormat="1" spans="4:15">
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -1850,32 +1854,32 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet6"/>
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
+  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="17.3653846153846" style="1" customWidth="1"/>
-    <col min="2" max="3" width="9.23076923076923" style="1"/>
-    <col min="4" max="7" width="9.23076923076923" style="2"/>
-    <col min="8" max="8" width="9.23076923076923" style="1"/>
-    <col min="9" max="9" width="10.0096153846154" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9.23076923076923" style="2"/>
-    <col min="12" max="12" width="9.23076923076923" style="1"/>
-    <col min="13" max="13" width="10.8653846153846" style="2" customWidth="1"/>
-    <col min="14" max="15" width="9.23076923076923" style="2"/>
-    <col min="16" max="16384" width="9.23076923076923" style="1"/>
+    <col min="1" max="1" width="17.3666666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.69166666666667" style="1"/>
+    <col min="3" max="3" width="9.23333333333333" style="1"/>
+    <col min="4" max="7" width="9.23333333333333" style="2"/>
+    <col min="8" max="8" width="9.23333333333333" style="1"/>
+    <col min="9" max="9" width="10.0083333333333" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9.23333333333333" style="2"/>
+    <col min="12" max="12" width="9.23333333333333" style="1"/>
+    <col min="13" max="13" width="10.8666666666667" style="2" customWidth="1"/>
+    <col min="14" max="15" width="9.23333333333333" style="2"/>
+    <col min="16" max="16384" width="9.23333333333333" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:15">
@@ -1883,7 +1887,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -1940,9 +1944,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="4:15">
+    <row r="3" s="1" customFormat="1" spans="1:15">
       <c r="D3" s="6">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>12</v>
@@ -1951,7 +1955,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" s="4">
         <v>1</v>
@@ -1971,7 +1975,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="4">
-        <v>10000</v>
+        <v>1000000</v>
       </c>
       <c r="D4" s="6">
         <v>8</v>
@@ -1983,7 +1987,7 @@
         <v>13</v>
       </c>
       <c r="G4" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I4" s="4">
         <v>0.5</v>
@@ -1992,7 +1996,7 @@
         <v>13</v>
       </c>
       <c r="K4" s="6">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
@@ -2000,13 +2004,13 @@
     </row>
     <row r="5" s="1" customFormat="1" spans="1:15">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>12</v>
@@ -2031,23 +2035,23 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:15">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>22</v>
+      <c r="A6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="D6" s="6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G6" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="4">
         <v>0</v>
@@ -2067,12 +2071,20 @@
         <v>20</v>
       </c>
       <c r="B7" s="3">
-        <v>3000</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+        <v>3500</v>
+      </c>
+      <c r="D7" s="6">
+        <v>8</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
       <c r="I7" s="4">
         <v>1.25</v>
       </c>
@@ -2086,13 +2098,13 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" s="1" customFormat="1" spans="4:15">
+    <row r="8" s="1" customFormat="1" spans="1:15">
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="I8" s="4">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>13</v>
@@ -2104,7 +2116,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" s="1" customFormat="1" spans="4:15">
+    <row r="9" s="1" customFormat="1" spans="1:15">
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -2116,27 +2128,35 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" s="1" customFormat="1" spans="4:15">
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+    <row r="10" s="1" customFormat="1" spans="1:15">
+      <c r="D10" s="6">
+        <v>6</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
       <c r="I10" s="4">
-        <v>2.1</v>
+        <v>0.875</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K10" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" s="1" customFormat="1" spans="4:15">
+    <row r="11" s="1" customFormat="1" spans="1:15">
       <c r="D11" s="6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>21</v>
@@ -2145,24 +2165,24 @@
         <v>13</v>
       </c>
       <c r="G11" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" s="4">
-        <v>1.95</v>
+        <v>1.375</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K11" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" s="1" customFormat="1" spans="4:15">
+    <row r="12" s="1" customFormat="1" spans="1:15">
       <c r="D12" s="6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>21</v>
@@ -2171,24 +2191,24 @@
         <v>13</v>
       </c>
       <c r="G12" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" s="4">
-        <v>1.6625</v>
+        <v>1.375</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K12" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" s="1" customFormat="1" spans="4:15">
+    <row r="13" s="1" customFormat="1" spans="1:15">
       <c r="D13" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>21</v>
@@ -2200,43 +2220,51 @@
         <v>0</v>
       </c>
       <c r="I13" s="4">
-        <v>1.375</v>
+        <v>1.1</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K13" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" s="1" customFormat="1" spans="4:15">
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+    <row r="14" s="1" customFormat="1" spans="1:15">
+      <c r="D14" s="6">
+        <v>2</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0</v>
+      </c>
       <c r="I14" s="4">
-        <v>1.1</v>
+        <v>0.8125</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>13</v>
       </c>
       <c r="K14" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" s="1" customFormat="1" spans="4:15">
+    <row r="15" s="1" customFormat="1" spans="1:15">
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="I15" s="4">
-        <v>0.8125</v>
+        <v>0.525</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>13</v>
@@ -2248,20 +2276,14 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" s="1" customFormat="1" spans="4:15">
+    <row r="16" s="1" customFormat="1" spans="1:15">
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="I16" s="4">
-        <v>0.525</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K16" s="6">
-        <v>0</v>
-      </c>
+      <c r="I16" s="4"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
@@ -2271,9 +2293,15 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
+      <c r="I17" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" s="6">
+        <v>0</v>
+      </c>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
@@ -2283,9 +2311,16 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
+      <c r="I18" s="4">
+        <f>0.8125-1</f>
+        <v>-0.1875</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" s="6">
+        <v>0</v>
+      </c>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
@@ -2408,26 +2443,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
+  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="17.3653846153846" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.69230769230769" style="1"/>
-    <col min="3" max="3" width="9.23076923076923" style="1"/>
-    <col min="4" max="7" width="9.23076923076923" style="2"/>
-    <col min="8" max="8" width="9.23076923076923" style="1"/>
-    <col min="9" max="9" width="10.0096153846154" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9.23076923076923" style="2"/>
-    <col min="12" max="12" width="9.23076923076923" style="1"/>
-    <col min="13" max="13" width="10.8653846153846" style="2" customWidth="1"/>
-    <col min="14" max="15" width="9.23076923076923" style="2"/>
-    <col min="16" max="16384" width="9.23076923076923" style="1"/>
+    <col min="1" max="1" width="17.3666666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.69166666666667" style="1"/>
+    <col min="3" max="3" width="9.23333333333333" style="1"/>
+    <col min="4" max="7" width="9.23333333333333" style="2"/>
+    <col min="8" max="8" width="9.23333333333333" style="1"/>
+    <col min="9" max="9" width="10.0083333333333" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9.23333333333333" style="2"/>
+    <col min="12" max="12" width="9.23333333333333" style="1"/>
+    <col min="13" max="13" width="10.8666666666667" style="2" customWidth="1"/>
+    <col min="14" max="15" width="9.23333333333333" style="2"/>
+    <col min="16" max="16384" width="9.23333333333333" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:15">
@@ -2435,7 +2470,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -2492,9 +2527,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="4:15">
+    <row r="3" s="1" customFormat="1" spans="1:15">
       <c r="D3" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>12</v>
@@ -2512,7 +2547,7 @@
         <v>13</v>
       </c>
       <c r="K3" s="6">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -2526,7 +2561,7 @@
         <v>1000000</v>
       </c>
       <c r="D4" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>12</v>
@@ -2538,7 +2573,7 @@
         <v>2</v>
       </c>
       <c r="I4" s="4">
-        <v>0.875</v>
+        <v>0.5</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>13</v>
@@ -2552,19 +2587,19 @@
     </row>
     <row r="5" s="1" customFormat="1" spans="1:15">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G5" s="6">
         <v>0</v>
@@ -2583,26 +2618,26 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:15">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>22</v>
+      <c r="A6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="D6" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
       </c>
       <c r="I6" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>13</v>
@@ -2619,14 +2654,22 @@
         <v>20</v>
       </c>
       <c r="B7" s="3">
-        <v>3000</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+        <v>3500</v>
+      </c>
+      <c r="D7" s="6">
+        <v>8</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
       <c r="I7" s="4">
-        <v>0.9</v>
+        <v>1.25</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>13</v>
@@ -2638,13 +2681,13 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" s="1" customFormat="1" spans="4:15">
+    <row r="8" s="1" customFormat="1" spans="1:15">
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="I8" s="4">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>13</v>
@@ -2656,7 +2699,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" s="1" customFormat="1" spans="4:15">
+    <row r="9" s="1" customFormat="1" spans="1:15">
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -2668,9 +2711,9 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" s="1" customFormat="1" spans="4:15">
+    <row r="10" s="1" customFormat="1" spans="1:15">
       <c r="D10" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>21</v>
@@ -2681,16 +2724,22 @@
       <c r="G10" s="6">
         <v>0</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="I10" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" s="1" customFormat="1" spans="4:15">
+    <row r="11" s="1" customFormat="1" spans="1:15">
       <c r="D11" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>21</v>
@@ -2702,7 +2751,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="4">
-        <v>1.6625</v>
+        <v>1.375</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>13</v>
@@ -2714,9 +2763,9 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" s="1" customFormat="1" spans="4:15">
+    <row r="12" s="1" customFormat="1" spans="1:15">
       <c r="D12" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>21</v>
@@ -2725,7 +2774,7 @@
         <v>13</v>
       </c>
       <c r="G12" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" s="4">
         <v>1.375</v>
@@ -2740,11 +2789,19 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" s="1" customFormat="1" spans="4:15">
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+    <row r="13" s="1" customFormat="1" spans="1:15">
+      <c r="D13" s="6">
+        <v>3</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0</v>
+      </c>
       <c r="I13" s="4">
         <v>1.1</v>
       </c>
@@ -2758,11 +2815,19 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" s="1" customFormat="1" spans="4:15">
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+    <row r="14" s="1" customFormat="1" spans="1:15">
+      <c r="D14" s="6">
+        <v>2</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0</v>
+      </c>
       <c r="I14" s="4">
         <v>0.8125</v>
       </c>
@@ -2776,7 +2841,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" s="1" customFormat="1" spans="4:15">
+    <row r="15" s="1" customFormat="1" spans="1:15">
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -2794,7 +2859,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" s="1" customFormat="1" spans="4:15">
+    <row r="16" s="1" customFormat="1" spans="1:15">
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -2811,9 +2876,15 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
+      <c r="I17" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" s="6">
+        <v>0</v>
+      </c>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
@@ -2823,9 +2894,16 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
+      <c r="I18" s="4">
+        <f>0.8125-1</f>
+        <v>-0.1875</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" s="6">
+        <v>0</v>
+      </c>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
@@ -2948,29 +3026,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet8"/>
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView zoomScale="204" zoomScaleNormal="204" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
+  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="17.3653846153846" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.69230769230769" style="1"/>
-    <col min="3" max="3" width="9.23076923076923" style="1"/>
-    <col min="4" max="7" width="9.23076923076923" style="2"/>
-    <col min="8" max="8" width="9.23076923076923" style="1"/>
-    <col min="9" max="9" width="10.0096153846154" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9.23076923076923" style="2"/>
-    <col min="12" max="12" width="9.23076923076923" style="1"/>
-    <col min="13" max="13" width="10.8653846153846" style="2" customWidth="1"/>
-    <col min="14" max="15" width="9.23076923076923" style="2"/>
-    <col min="16" max="16384" width="9.23076923076923" style="1"/>
+    <col min="1" max="1" width="17.3666666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.69166666666667" style="1"/>
+    <col min="3" max="3" width="9.23333333333333" style="1"/>
+    <col min="4" max="7" width="9.23333333333333" style="2"/>
+    <col min="8" max="8" width="9.23333333333333" style="1"/>
+    <col min="9" max="9" width="10.0083333333333" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9.23333333333333" style="2"/>
+    <col min="12" max="12" width="9.23333333333333" style="1"/>
+    <col min="13" max="13" width="10.8666666666667" style="2" customWidth="1"/>
+    <col min="14" max="15" width="9.23333333333333" style="2"/>
+    <col min="16" max="16384" width="9.23333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:15">
+    <row r="1" spans="1:15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2994,7 +3072,7 @@
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:15">
+    <row r="2" spans="1:15">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -3032,7 +3110,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="4:15">
+    <row r="3" spans="1:15">
       <c r="D3" s="6">
         <v>7</v>
       </c>
@@ -3052,18 +3130,18 @@
         <v>13</v>
       </c>
       <c r="K3" s="6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" s="1" customFormat="1" spans="1:15">
+    <row r="4" spans="1:15">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="4">
-        <v>500000</v>
+        <v>1000000</v>
       </c>
       <c r="D4" s="6">
         <v>6</v>
@@ -3090,12 +3168,12 @@
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
     </row>
-    <row r="5" s="1" customFormat="1" spans="1:15">
+    <row r="5" spans="1:15">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="6">
         <v>5</v>
@@ -3104,7 +3182,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G5" s="6">
         <v>0</v>
@@ -3122,12 +3200,12 @@
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
     </row>
-    <row r="6" s="1" customFormat="1" spans="1:15">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>22</v>
+    <row r="6" spans="1:15">
+      <c r="A6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="D6" s="6">
         <v>5</v>
@@ -3136,7 +3214,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
@@ -3154,7 +3232,7 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:15">
+    <row r="7" spans="1:15">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -3186,7 +3264,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" s="1" customFormat="1" spans="4:15">
+    <row r="8" spans="1:15">
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -3204,7 +3282,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" s="1" customFormat="1" spans="4:15">
+    <row r="9" spans="1:15">
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -3216,7 +3294,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" s="1" customFormat="1" spans="4:15">
+    <row r="10" spans="1:15">
       <c r="D10" s="6">
         <v>6</v>
       </c>
@@ -3242,7 +3320,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" s="1" customFormat="1" spans="4:15">
+    <row r="11" spans="1:15">
       <c r="D11" s="6">
         <v>5</v>
       </c>
@@ -3253,7 +3331,7 @@
         <v>13</v>
       </c>
       <c r="G11" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" s="4">
         <v>1.375</v>
@@ -3268,7 +3346,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" s="1" customFormat="1" spans="4:15">
+    <row r="12" spans="1:15">
       <c r="D12" s="6">
         <v>4</v>
       </c>
@@ -3294,7 +3372,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" s="1" customFormat="1" spans="4:15">
+    <row r="13" spans="1:15">
       <c r="D13" s="6">
         <v>3</v>
       </c>
@@ -3320,7 +3398,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" s="1" customFormat="1" spans="4:15">
+    <row r="14" spans="1:15">
       <c r="D14" s="6">
         <v>2</v>
       </c>
@@ -3346,7 +3424,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" s="1" customFormat="1" spans="4:15">
+    <row r="15" spans="1:15">
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -3364,7 +3442,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" s="1" customFormat="1" spans="4:15">
+    <row r="16" spans="1:15">
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -3376,7 +3454,7 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" s="1" customFormat="1" spans="4:15">
+    <row r="17" spans="4:15">
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -3394,7 +3472,7 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" s="1" customFormat="1" spans="4:15">
+    <row r="18" spans="4:15">
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -3413,7 +3491,7 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
     </row>
-    <row r="19" s="1" customFormat="1" spans="4:15">
+    <row r="19" spans="4:15">
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -3425,7 +3503,7 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
     </row>
-    <row r="20" s="1" customFormat="1" spans="4:15">
+    <row r="20" spans="4:15">
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -3437,7 +3515,7 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
     </row>
-    <row r="21" s="1" customFormat="1" spans="4:15">
+    <row r="21" spans="4:15">
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -3449,7 +3527,7 @@
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
     </row>
-    <row r="22" s="1" customFormat="1" spans="4:15">
+    <row r="22" spans="4:15">
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -3461,7 +3539,7 @@
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
     </row>
-    <row r="23" s="1" customFormat="1" spans="4:15">
+    <row r="23" spans="4:15">
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -3473,7 +3551,7 @@
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
     </row>
-    <row r="24" s="1" customFormat="1" spans="4:15">
+    <row r="24" spans="4:15">
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -3485,7 +3563,7 @@
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
     </row>
-    <row r="25" s="1" customFormat="1" spans="4:15">
+    <row r="25" spans="4:15">
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -3531,25 +3609,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet34"/>
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
+  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="17.3653846153846" style="1" customWidth="1"/>
-    <col min="2" max="3" width="9.23076923076923" style="1"/>
-    <col min="4" max="7" width="9.23076923076923" style="2"/>
-    <col min="8" max="8" width="9.23076923076923" style="1"/>
-    <col min="9" max="9" width="10.0096153846154" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9.23076923076923" style="2"/>
-    <col min="12" max="12" width="9.23076923076923" style="1"/>
-    <col min="13" max="13" width="10.8653846153846" style="2" customWidth="1"/>
-    <col min="14" max="15" width="9.23076923076923" style="2"/>
-    <col min="16" max="16384" width="9.23076923076923" style="1"/>
+    <col min="1" max="1" width="17.3666666666667" style="1" customWidth="1"/>
+    <col min="2" max="3" width="9.23333333333333" style="1"/>
+    <col min="4" max="7" width="9.23333333333333" style="2"/>
+    <col min="8" max="8" width="9.23333333333333" style="1"/>
+    <col min="9" max="9" width="10.0083333333333" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9.23333333333333" style="2"/>
+    <col min="12" max="12" width="9.23333333333333" style="1"/>
+    <col min="13" max="13" width="10.8666666666667" style="2" customWidth="1"/>
+    <col min="14" max="15" width="9.23333333333333" style="2"/>
+    <col min="16" max="16384" width="9.23333333333333" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:15">
@@ -3557,7 +3635,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -3614,7 +3692,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="4:15">
+    <row r="3" s="1" customFormat="1" spans="1:15">
       <c r="D3" s="6">
         <v>9</v>
       </c>
@@ -3625,7 +3703,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="4">
         <v>1</v>
@@ -3634,7 +3712,7 @@
         <v>13</v>
       </c>
       <c r="K3" s="6">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -3645,7 +3723,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="4">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="D4" s="6">
         <v>8</v>
@@ -3657,7 +3735,7 @@
         <v>13</v>
       </c>
       <c r="G4" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I4" s="4">
         <v>0.5</v>
@@ -3666,7 +3744,7 @@
         <v>13</v>
       </c>
       <c r="K4" s="6">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
@@ -3674,10 +3752,10 @@
     </row>
     <row r="5" s="1" customFormat="1" spans="1:15">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="6">
         <v>7</v>
@@ -3689,7 +3767,7 @@
         <v>13</v>
       </c>
       <c r="G5" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I5" s="4">
         <v>0.25</v>
@@ -3705,23 +3783,23 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:15">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>22</v>
+      <c r="A6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="D6" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G6" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="4">
         <v>0</v>
@@ -3741,20 +3819,12 @@
         <v>20</v>
       </c>
       <c r="B7" s="3">
-        <v>1700</v>
-      </c>
-      <c r="D7" s="6">
-        <v>5</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="6">
-        <v>0</v>
-      </c>
+        <v>3000</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
       <c r="I7" s="4">
         <v>1.25</v>
       </c>
@@ -3768,19 +3838,11 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" s="1" customFormat="1" spans="4:15">
-      <c r="D8" s="6">
-        <v>5</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="6">
-        <v>0</v>
-      </c>
+    <row r="8" s="1" customFormat="1" spans="1:15">
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
       <c r="I8" s="4">
         <v>1.5</v>
       </c>
@@ -3794,7 +3856,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" s="1" customFormat="1" spans="4:15">
+    <row r="9" s="1" customFormat="1" spans="1:15">
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -3806,7 +3868,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" s="1" customFormat="1" spans="4:15">
+    <row r="10" s="1" customFormat="1" spans="1:15">
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -3818,15 +3880,15 @@
         <v>13</v>
       </c>
       <c r="K10" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" s="1" customFormat="1" spans="4:15">
+    <row r="11" s="1" customFormat="1" spans="1:15">
       <c r="D11" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>21</v>
@@ -3835,7 +3897,7 @@
         <v>13</v>
       </c>
       <c r="G11" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="4">
         <v>1.95</v>
@@ -3844,15 +3906,15 @@
         <v>13</v>
       </c>
       <c r="K11" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" s="1" customFormat="1" spans="4:15">
+    <row r="12" s="1" customFormat="1" spans="1:15">
       <c r="D12" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>21</v>
@@ -3861,7 +3923,7 @@
         <v>13</v>
       </c>
       <c r="G12" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="4">
         <v>1.6625</v>
@@ -3870,15 +3932,15 @@
         <v>13</v>
       </c>
       <c r="K12" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" s="1" customFormat="1" spans="4:15">
+    <row r="13" s="1" customFormat="1" spans="1:15">
       <c r="D13" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>21</v>
@@ -3896,25 +3958,17 @@
         <v>13</v>
       </c>
       <c r="K13" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" s="1" customFormat="1" spans="4:15">
-      <c r="D14" s="6">
-        <v>3</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="6">
-        <v>0</v>
-      </c>
+    <row r="14" s="1" customFormat="1" spans="1:15">
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
       <c r="I14" s="4">
         <v>1.1</v>
       </c>
@@ -3922,13 +3976,13 @@
         <v>13</v>
       </c>
       <c r="K14" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" s="1" customFormat="1" spans="4:15">
+    <row r="15" s="1" customFormat="1" spans="1:15">
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -3946,7 +4000,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" s="1" customFormat="1" spans="4:15">
+    <row r="16" s="1" customFormat="1" spans="1:15">
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -4106,25 +4160,25 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet4"/>
+  <sheetPr codeName="Sheet34"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
+  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="17.3653846153846" style="1" customWidth="1"/>
-    <col min="2" max="3" width="9.23076923076923" style="1"/>
-    <col min="4" max="7" width="9.23076923076923" style="2"/>
-    <col min="8" max="8" width="9.23076923076923" style="1"/>
-    <col min="9" max="9" width="10.0096153846154" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9.23076923076923" style="2"/>
-    <col min="12" max="12" width="9.23076923076923" style="1"/>
-    <col min="13" max="13" width="10.8653846153846" style="2" customWidth="1"/>
-    <col min="14" max="15" width="9.23076923076923" style="2"/>
-    <col min="16" max="16384" width="9.23076923076923" style="1"/>
+    <col min="1" max="1" width="17.3666666666667" style="1" customWidth="1"/>
+    <col min="2" max="3" width="9.23333333333333" style="1"/>
+    <col min="4" max="7" width="9.23333333333333" style="2"/>
+    <col min="8" max="8" width="9.23333333333333" style="1"/>
+    <col min="9" max="9" width="10.0083333333333" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9.23333333333333" style="2"/>
+    <col min="12" max="12" width="9.23333333333333" style="1"/>
+    <col min="13" max="13" width="10.8666666666667" style="2" customWidth="1"/>
+    <col min="14" max="15" width="9.23333333333333" style="2"/>
+    <col min="16" max="16384" width="9.23333333333333" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:15">
@@ -4132,7 +4186,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -4189,9 +4243,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="4:15">
+    <row r="3" s="1" customFormat="1" spans="1:15">
       <c r="D3" s="6">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>12</v>
@@ -4200,7 +4254,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" s="4">
         <v>1</v>
@@ -4209,7 +4263,7 @@
         <v>13</v>
       </c>
       <c r="K3" s="6">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -4220,10 +4274,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="4">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="D4" s="6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>12</v>
@@ -4249,22 +4303,22 @@
     </row>
     <row r="5" s="1" customFormat="1" spans="1:15">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="6">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G5" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I5" s="4">
         <v>0.25</v>
@@ -4280,20 +4334,20 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:15">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>22</v>
+      <c r="A6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="D6" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
@@ -4316,16 +4370,16 @@
         <v>20</v>
       </c>
       <c r="B7" s="3">
-        <v>3000</v>
+        <v>1700</v>
       </c>
       <c r="D7" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G7" s="6">
         <v>0</v>
@@ -4343,11 +4397,19 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" s="1" customFormat="1" spans="4:15">
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+    <row r="8" s="1" customFormat="1" spans="1:15">
+      <c r="D8" s="6">
+        <v>5</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
       <c r="I8" s="4">
         <v>1.5</v>
       </c>
@@ -4361,7 +4423,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" s="1" customFormat="1" spans="4:15">
+    <row r="9" s="1" customFormat="1" spans="1:15">
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -4373,7 +4435,574 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" s="1" customFormat="1" spans="4:15">
+    <row r="10" s="1" customFormat="1" spans="1:15">
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="I10" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" s="1" customFormat="1" spans="1:15">
+      <c r="D11" s="6">
+        <v>6</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1.95</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0</v>
+      </c>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" s="1" customFormat="1" spans="1:15">
+      <c r="D12" s="6">
+        <v>5</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>1.6625</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0</v>
+      </c>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" s="1" customFormat="1" spans="1:15">
+      <c r="D13" s="6">
+        <v>4</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>1.375</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0</v>
+      </c>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+    </row>
+    <row r="14" s="1" customFormat="1" spans="1:15">
+      <c r="D14" s="6">
+        <v>3</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>1.1</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0</v>
+      </c>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+    </row>
+    <row r="15" s="1" customFormat="1" spans="1:15">
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="I15" s="4">
+        <v>0.8125</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" s="6">
+        <v>0</v>
+      </c>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+    </row>
+    <row r="16" s="1" customFormat="1" spans="1:15">
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="I16" s="4">
+        <v>0.525</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" s="6">
+        <v>0</v>
+      </c>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+    </row>
+    <row r="17" s="1" customFormat="1" spans="4:15">
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+    </row>
+    <row r="18" s="1" customFormat="1" spans="4:15">
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+    </row>
+    <row r="19" s="1" customFormat="1" spans="4:15">
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+    </row>
+    <row r="20" s="1" customFormat="1" spans="4:15">
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+    </row>
+    <row r="21" s="1" customFormat="1" spans="4:15">
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" s="1" customFormat="1" spans="4:15">
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+    </row>
+    <row r="23" s="1" customFormat="1" spans="4:15">
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+    </row>
+    <row r="24" s="1" customFormat="1" spans="4:15">
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" s="1" customFormat="1" spans="4:15">
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M1:O1"/>
+  </mergeCells>
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"普通,南瓜,冰道,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"是,否"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"随机,最快,最慢"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+      <formula1>"曾,喷"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25 J3:J25 N3:N25">
+      <formula1>"永动,非永动"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:O25"/>
+  <sheetViews>
+    <sheetView zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="17.3666666666667" style="1" customWidth="1"/>
+    <col min="2" max="3" width="9.23333333333333" style="1"/>
+    <col min="4" max="7" width="9.23333333333333" style="2"/>
+    <col min="8" max="8" width="9.23333333333333" style="1"/>
+    <col min="9" max="9" width="10.0083333333333" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9.23333333333333" style="2"/>
+    <col min="12" max="12" width="9.23333333333333" style="1"/>
+    <col min="13" max="13" width="10.8666666666667" style="2" customWidth="1"/>
+    <col min="14" max="15" width="9.23333333333333" style="2"/>
+    <col min="16" max="16384" width="9.23333333333333" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:15">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4">
+        <v>4</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="I1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="M1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:15">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:15">
+      <c r="D3" s="6">
+        <v>5</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+    </row>
+    <row r="4" s="1" customFormat="1" spans="1:15">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="4">
+        <v>10000</v>
+      </c>
+      <c r="D4" s="6">
+        <v>4</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:15">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="6">
+        <v>4</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:15">
+      <c r="A6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="6">
+        <v>3</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:15">
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3000</v>
+      </c>
+      <c r="D7" s="6">
+        <v>3</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1.25</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0</v>
+      </c>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" s="1" customFormat="1" spans="1:15">
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="I8" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" s="1" customFormat="1" spans="1:15">
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+    </row>
+    <row r="10" s="1" customFormat="1" spans="1:15">
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -4391,7 +5020,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" s="1" customFormat="1" spans="4:15">
+    <row r="11" s="1" customFormat="1" spans="1:15">
       <c r="D11" s="6">
         <v>4</v>
       </c>
@@ -4417,7 +5046,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" s="1" customFormat="1" spans="4:15">
+    <row r="12" s="1" customFormat="1" spans="1:15">
       <c r="D12" s="6">
         <v>3</v>
       </c>
@@ -4443,7 +5072,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" s="1" customFormat="1" spans="4:15">
+    <row r="13" s="1" customFormat="1" spans="1:15">
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -4451,7 +5080,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G13" s="6">
         <v>0</v>
@@ -4469,7 +5098,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" s="1" customFormat="1" spans="4:15">
+    <row r="14" s="1" customFormat="1" spans="1:15">
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -4481,7 +5110,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" s="1" customFormat="1" spans="4:15">
+    <row r="15" s="1" customFormat="1" spans="1:15">
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -4493,7 +5122,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" s="1" customFormat="1" spans="4:15">
+    <row r="16" s="1" customFormat="1" spans="1:15">
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>

</xml_diff>

<commit_message>
modified:   Zomboni/zomboni_test_info.xlsx 	modified:   inc/tools/Zomboni.hpp
</commit_message>
<xml_diff>
--- a/Zomboni/zomboni_test_info.xlsx
+++ b/Zomboni/zomboni_test_info.xlsx
@@ -7,9 +7,9 @@
     <workbookView windowWidth="27750" windowHeight="10665"/>
   </bookViews>
   <sheets>
-    <sheet name="守一" sheetId="9" r:id="rId1"/>
-    <sheet name="守五" sheetId="8" r:id="rId2"/>
-    <sheet name="tmp" sheetId="4" r:id="rId3"/>
+    <sheet name="tmp" sheetId="4" r:id="rId1"/>
+    <sheet name="守一" sheetId="9" r:id="rId2"/>
+    <sheet name="守五" sheetId="8" r:id="rId3"/>
     <sheet name="守六" sheetId="1" r:id="rId4"/>
     <sheet name="守八" sheetId="2" r:id="rId5"/>
     <sheet name="守七" sheetId="7" r:id="rId6"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="23">
   <si>
     <t>被压列数</t>
   </si>
@@ -74,13 +74,13 @@
     <t>曾</t>
   </si>
   <si>
+    <t>非永动</t>
+  </si>
+  <si>
     <t>永动</t>
   </si>
   <si>
     <t>测试次数</t>
-  </si>
-  <si>
-    <t>非永动</t>
   </si>
   <si>
     <t>是否展示测试进度</t>
@@ -92,13 +92,16 @@
     <t>锁植物攻击间隔</t>
   </si>
   <si>
-    <t>随机</t>
+    <t>最慢</t>
   </si>
   <si>
     <t>时间上限</t>
   </si>
   <si>
     <t>喷</t>
+  </si>
+  <si>
+    <t>随机</t>
   </si>
 </sst>
 </file>
@@ -1278,11 +1281,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
@@ -1305,7 +1308,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -1364,7 +1367,7 @@
     </row>
     <row r="3" s="1" customFormat="1" spans="1:15">
       <c r="D3" s="6">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>12</v>
@@ -1373,13 +1376,13 @@
         <v>13</v>
       </c>
       <c r="G3" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="4">
         <v>1</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K3" s="6">
         <v>0</v>
@@ -1390,28 +1393,28 @@
     </row>
     <row r="4" s="1" customFormat="1" spans="1:15">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4">
         <v>1000000</v>
       </c>
       <c r="D4" s="6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="4">
         <v>0.5</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K4" s="6">
         <v>0</v>
@@ -1428,22 +1431,22 @@
         <v>17</v>
       </c>
       <c r="D5" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G5" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I5" s="4">
         <v>0.25</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K5" s="6">
         <v>0</v>
@@ -1466,7 +1469,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
@@ -1475,7 +1478,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K6" s="6">
         <v>0</v>
@@ -1498,7 +1501,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G7" s="6">
         <v>0</v>
@@ -1507,7 +1510,7 @@
         <v>1.25</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K7" s="6">
         <v>0</v>
@@ -1525,7 +1528,7 @@
         <v>2</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K8" s="6">
         <v>0</v>
@@ -1554,7 +1557,7 @@
         <v>21</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G10" s="6">
         <v>0</v>
@@ -1563,7 +1566,7 @@
         <v>0.875</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K10" s="6">
         <v>0</v>
@@ -1580,7 +1583,7 @@
         <v>21</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G11" s="6">
         <v>0</v>
@@ -1589,7 +1592,7 @@
         <v>1.375</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K11" s="6">
         <v>0</v>
@@ -1606,7 +1609,7 @@
         <v>21</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G12" s="6">
         <v>0</v>
@@ -1615,7 +1618,7 @@
         <v>1.375</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K12" s="6">
         <v>0</v>
@@ -1632,7 +1635,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G13" s="6">
         <v>0</v>
@@ -1641,7 +1644,7 @@
         <v>1.1</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K13" s="6">
         <v>0</v>
@@ -1658,7 +1661,7 @@
         <v>21</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G14" s="6">
         <v>0</v>
@@ -1667,7 +1670,7 @@
         <v>0.8125</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K14" s="6">
         <v>0</v>
@@ -1685,7 +1688,7 @@
         <v>0.525</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K15" s="6">
         <v>0</v>
@@ -1715,7 +1718,7 @@
         <v>0.1</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K17" s="6">
         <v>0</v>
@@ -1734,7 +1737,7 @@
         <v>-0.1875</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K18" s="6">
         <v>0</v>
@@ -1833,9 +1836,9 @@
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="M1:O1"/>
   </mergeCells>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"0,1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>"普通,南瓜,冰道,炮"</formula1>
@@ -1846,6 +1849,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
       <formula1>"随机,最快,最慢"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
       <formula1>"曾,喷"</formula1>
     </dataValidation>
@@ -1854,17 +1860,18 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
@@ -1887,7 +1894,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -1952,7 +1959,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="6">
         <v>0</v>
@@ -1961,7 +1968,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K3" s="6">
         <v>0</v>
@@ -1972,13 +1979,13 @@
     </row>
     <row r="4" s="1" customFormat="1" spans="1:15">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4">
         <v>1000000</v>
       </c>
       <c r="D4" s="6">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>12</v>
@@ -1993,7 +2000,7 @@
         <v>0.5</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K4" s="6">
         <v>0</v>
@@ -2010,7 +2017,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>12</v>
@@ -2019,13 +2026,13 @@
         <v>13</v>
       </c>
       <c r="G5" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I5" s="4">
         <v>0.25</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K5" s="6">
         <v>0</v>
@@ -2039,7 +2046,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D6" s="6">
         <v>5</v>
@@ -2048,7 +2055,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
@@ -2057,7 +2064,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K6" s="6">
         <v>0</v>
@@ -2080,7 +2087,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G7" s="6">
         <v>0</v>
@@ -2089,7 +2096,7 @@
         <v>1.25</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K7" s="6">
         <v>0</v>
@@ -2107,7 +2114,7 @@
         <v>2</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K8" s="6">
         <v>0</v>
@@ -2136,7 +2143,7 @@
         <v>21</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G10" s="6">
         <v>0</v>
@@ -2145,7 +2152,7 @@
         <v>0.875</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K10" s="6">
         <v>0</v>
@@ -2162,7 +2169,7 @@
         <v>21</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G11" s="6">
         <v>0</v>
@@ -2171,7 +2178,7 @@
         <v>1.375</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K11" s="6">
         <v>0</v>
@@ -2188,7 +2195,7 @@
         <v>21</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G12" s="6">
         <v>0</v>
@@ -2197,7 +2204,7 @@
         <v>1.375</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K12" s="6">
         <v>0</v>
@@ -2214,7 +2221,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G13" s="6">
         <v>0</v>
@@ -2223,7 +2230,7 @@
         <v>1.1</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K13" s="6">
         <v>0</v>
@@ -2240,7 +2247,7 @@
         <v>21</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G14" s="6">
         <v>0</v>
@@ -2249,7 +2256,7 @@
         <v>0.8125</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K14" s="6">
         <v>0</v>
@@ -2267,7 +2274,7 @@
         <v>0.525</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K15" s="6">
         <v>0</v>
@@ -2297,7 +2304,7 @@
         <v>0.1</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K17" s="6">
         <v>0</v>
@@ -2316,7 +2323,7 @@
         <v>-0.1875</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K18" s="6">
         <v>0</v>
@@ -2415,9 +2422,9 @@
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="M1:O1"/>
   </mergeCells>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"0,1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>"普通,南瓜,冰道,炮"</formula1>
@@ -2428,6 +2435,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
       <formula1>"随机,最快,最慢"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
       <formula1>"曾,喷"</formula1>
     </dataValidation>
@@ -2436,18 +2446,17 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet8"/>
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+    <sheetView zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
@@ -2470,7 +2479,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -2535,7 +2544,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="6">
         <v>0</v>
@@ -2544,10 +2553,10 @@
         <v>1</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K3" s="6">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -2555,28 +2564,28 @@
     </row>
     <row r="4" s="1" customFormat="1" spans="1:15">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4">
         <v>1000000</v>
       </c>
       <c r="D4" s="6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4" s="4">
         <v>0.5</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K4" s="6">
         <v>0</v>
@@ -2599,16 +2608,16 @@
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="4">
         <v>0.25</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K5" s="6">
         <v>0</v>
@@ -2622,7 +2631,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D6" s="6">
         <v>5</v>
@@ -2631,7 +2640,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
@@ -2640,7 +2649,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K6" s="6">
         <v>0</v>
@@ -2663,7 +2672,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G7" s="6">
         <v>0</v>
@@ -2672,7 +2681,7 @@
         <v>1.25</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K7" s="6">
         <v>0</v>
@@ -2690,7 +2699,7 @@
         <v>2</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K8" s="6">
         <v>0</v>
@@ -2719,7 +2728,7 @@
         <v>21</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G10" s="6">
         <v>0</v>
@@ -2728,7 +2737,7 @@
         <v>0.875</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K10" s="6">
         <v>0</v>
@@ -2745,16 +2754,16 @@
         <v>21</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G11" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" s="4">
         <v>1.375</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K11" s="6">
         <v>0</v>
@@ -2771,7 +2780,7 @@
         <v>21</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G12" s="6">
         <v>0</v>
@@ -2780,7 +2789,7 @@
         <v>1.375</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K12" s="6">
         <v>0</v>
@@ -2797,7 +2806,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G13" s="6">
         <v>0</v>
@@ -2806,7 +2815,7 @@
         <v>1.1</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K13" s="6">
         <v>0</v>
@@ -2823,7 +2832,7 @@
         <v>21</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G14" s="6">
         <v>0</v>
@@ -2832,7 +2841,7 @@
         <v>0.8125</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K14" s="6">
         <v>0</v>
@@ -2850,7 +2859,7 @@
         <v>0.525</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K15" s="6">
         <v>0</v>
@@ -2880,7 +2889,7 @@
         <v>0.1</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K17" s="6">
         <v>0</v>
@@ -2899,7 +2908,7 @@
         <v>-0.1875</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K18" s="6">
         <v>0</v>
@@ -2998,9 +3007,9 @@
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="M1:O1"/>
   </mergeCells>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"0,1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>"普通,南瓜,冰道,炮"</formula1>
@@ -3010,6 +3019,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
       <formula1>"随机,最快,最慢"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
       <formula1>"曾,喷"</formula1>
@@ -3030,7 +3042,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
@@ -3118,7 +3130,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="6">
         <v>0</v>
@@ -3127,7 +3139,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K3" s="6">
         <v>8</v>
@@ -3138,7 +3150,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4">
         <v>1000000</v>
@@ -3150,7 +3162,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" s="6">
         <v>3</v>
@@ -3159,7 +3171,7 @@
         <v>0.5</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K4" s="6">
         <v>0</v>
@@ -3182,7 +3194,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G5" s="6">
         <v>0</v>
@@ -3191,7 +3203,7 @@
         <v>0.25</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K5" s="6">
         <v>0</v>
@@ -3205,7 +3217,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D6" s="6">
         <v>5</v>
@@ -3214,7 +3226,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
@@ -3223,7 +3235,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K6" s="6">
         <v>0</v>
@@ -3246,7 +3258,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G7" s="6">
         <v>0</v>
@@ -3255,7 +3267,7 @@
         <v>1.25</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K7" s="6">
         <v>0</v>
@@ -3273,7 +3285,7 @@
         <v>2</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K8" s="6">
         <v>0</v>
@@ -3302,7 +3314,7 @@
         <v>21</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G10" s="6">
         <v>0</v>
@@ -3311,7 +3323,7 @@
         <v>0.875</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K10" s="6">
         <v>0</v>
@@ -3328,7 +3340,7 @@
         <v>21</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G11" s="6">
         <v>0</v>
@@ -3337,7 +3349,7 @@
         <v>1.375</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K11" s="6">
         <v>0</v>
@@ -3354,7 +3366,7 @@
         <v>21</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G12" s="6">
         <v>0</v>
@@ -3363,7 +3375,7 @@
         <v>1.375</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K12" s="6">
         <v>0</v>
@@ -3380,7 +3392,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G13" s="6">
         <v>0</v>
@@ -3389,7 +3401,7 @@
         <v>1.1</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K13" s="6">
         <v>0</v>
@@ -3406,7 +3418,7 @@
         <v>21</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G14" s="6">
         <v>0</v>
@@ -3415,7 +3427,7 @@
         <v>0.8125</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K14" s="6">
         <v>0</v>
@@ -3433,7 +3445,7 @@
         <v>0.525</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K15" s="6">
         <v>0</v>
@@ -3463,7 +3475,7 @@
         <v>0.1</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K17" s="6">
         <v>0</v>
@@ -3482,7 +3494,7 @@
         <v>-0.1875</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K18" s="6">
         <v>0</v>
@@ -3581,9 +3593,9 @@
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="M1:O1"/>
   </mergeCells>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"0,1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>"普通,南瓜,冰道,炮"</formula1>
@@ -3593,6 +3605,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
       <formula1>"随机,最快,最慢"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
       <formula1>"曾,喷"</formula1>
@@ -3613,7 +3628,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
@@ -3700,7 +3715,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="6">
         <v>1</v>
@@ -3709,7 +3724,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K3" s="6">
         <v>0</v>
@@ -3720,7 +3735,7 @@
     </row>
     <row r="4" s="1" customFormat="1" spans="1:15">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4">
         <v>10000</v>
@@ -3732,7 +3747,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" s="6">
         <v>3</v>
@@ -3741,7 +3756,7 @@
         <v>0.5</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K4" s="6">
         <v>9</v>
@@ -3764,7 +3779,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G5" s="6">
         <v>1</v>
@@ -3773,7 +3788,7 @@
         <v>0.25</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K5" s="6">
         <v>0</v>
@@ -3787,7 +3802,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D6" s="6">
         <v>7</v>
@@ -3796,7 +3811,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G6" s="6">
         <v>1</v>
@@ -3805,7 +3820,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K6" s="6">
         <v>0</v>
@@ -3829,7 +3844,7 @@
         <v>1.25</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K7" s="6">
         <v>0</v>
@@ -3847,7 +3862,7 @@
         <v>1.5</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K8" s="6">
         <v>0</v>
@@ -3877,7 +3892,7 @@
         <v>2.1</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K10" s="6">
         <v>1</v>
@@ -3894,7 +3909,7 @@
         <v>21</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G11" s="6">
         <v>1</v>
@@ -3903,7 +3918,7 @@
         <v>1.95</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K11" s="6">
         <v>1</v>
@@ -3920,7 +3935,7 @@
         <v>21</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G12" s="6">
         <v>1</v>
@@ -3929,7 +3944,7 @@
         <v>1.6625</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K12" s="6">
         <v>1</v>
@@ -3946,7 +3961,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G13" s="6">
         <v>0</v>
@@ -3955,7 +3970,7 @@
         <v>1.375</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K13" s="6">
         <v>2</v>
@@ -3973,7 +3988,7 @@
         <v>1.1</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K14" s="6">
         <v>1</v>
@@ -3991,7 +4006,7 @@
         <v>0.8125</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K15" s="6">
         <v>0</v>
@@ -4009,7 +4024,7 @@
         <v>0.525</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K16" s="6">
         <v>0</v>
@@ -4132,9 +4147,9 @@
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="M1:O1"/>
   </mergeCells>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"0,1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>"普通,南瓜,冰道,炮"</formula1>
@@ -4144,6 +4159,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
       <formula1>"随机,最快,最慢"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
       <formula1>"曾,喷"</formula1>
@@ -4164,7 +4182,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
@@ -4251,7 +4269,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="6">
         <v>0</v>
@@ -4260,7 +4278,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K3" s="6">
         <v>13</v>
@@ -4271,7 +4289,7 @@
     </row>
     <row r="4" s="1" customFormat="1" spans="1:15">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4">
         <v>100000</v>
@@ -4283,7 +4301,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" s="6">
         <v>0</v>
@@ -4292,7 +4310,7 @@
         <v>0.5</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K4" s="6">
         <v>0</v>
@@ -4315,7 +4333,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G5" s="6">
         <v>3</v>
@@ -4324,7 +4342,7 @@
         <v>0.25</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K5" s="6">
         <v>0</v>
@@ -4338,7 +4356,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D6" s="6">
         <v>6</v>
@@ -4347,7 +4365,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
@@ -4356,7 +4374,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K6" s="6">
         <v>0</v>
@@ -4379,7 +4397,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G7" s="6">
         <v>0</v>
@@ -4388,7 +4406,7 @@
         <v>1.25</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K7" s="6">
         <v>0</v>
@@ -4405,7 +4423,7 @@
         <v>12</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G8" s="6">
         <v>0</v>
@@ -4414,7 +4432,7 @@
         <v>1.5</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K8" s="6">
         <v>0</v>
@@ -4444,7 +4462,7 @@
         <v>2.1</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K10" s="6">
         <v>0</v>
@@ -4461,7 +4479,7 @@
         <v>21</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G11" s="6">
         <v>0</v>
@@ -4470,7 +4488,7 @@
         <v>1.95</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K11" s="6">
         <v>0</v>
@@ -4487,7 +4505,7 @@
         <v>21</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G12" s="6">
         <v>0</v>
@@ -4496,7 +4514,7 @@
         <v>1.6625</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K12" s="6">
         <v>0</v>
@@ -4513,7 +4531,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G13" s="6">
         <v>0</v>
@@ -4522,7 +4540,7 @@
         <v>1.375</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K13" s="6">
         <v>0</v>
@@ -4539,7 +4557,7 @@
         <v>21</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G14" s="6">
         <v>0</v>
@@ -4548,7 +4566,7 @@
         <v>1.1</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K14" s="6">
         <v>0</v>
@@ -4566,7 +4584,7 @@
         <v>0.8125</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K15" s="6">
         <v>0</v>
@@ -4584,7 +4602,7 @@
         <v>0.525</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K16" s="6">
         <v>0</v>
@@ -4707,9 +4725,9 @@
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="M1:O1"/>
   </mergeCells>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"0,1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>"普通,南瓜,冰道,炮"</formula1>
@@ -4719,6 +4737,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
       <formula1>"随机,最快,最慢"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
       <formula1>"曾,喷"</formula1>
@@ -4739,7 +4760,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
@@ -4826,7 +4847,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="6">
         <v>1</v>
@@ -4835,7 +4856,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K3" s="6">
         <v>0</v>
@@ -4846,7 +4867,7 @@
     </row>
     <row r="4" s="1" customFormat="1" spans="1:15">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4">
         <v>10000</v>
@@ -4858,7 +4879,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" s="6">
         <v>0</v>
@@ -4867,7 +4888,7 @@
         <v>0.5</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K4" s="6">
         <v>0</v>
@@ -4890,7 +4911,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G5" s="6">
         <v>0</v>
@@ -4899,7 +4920,7 @@
         <v>0.25</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K5" s="6">
         <v>0</v>
@@ -4913,7 +4934,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D6" s="6">
         <v>3</v>
@@ -4922,7 +4943,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
@@ -4931,7 +4952,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K6" s="6">
         <v>0</v>
@@ -4954,7 +4975,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G7" s="6">
         <v>0</v>
@@ -4963,7 +4984,7 @@
         <v>1.25</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K7" s="6">
         <v>0</v>
@@ -4981,7 +5002,7 @@
         <v>1.5</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K8" s="6">
         <v>0</v>
@@ -5011,7 +5032,7 @@
         <v>1.375</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K10" s="6">
         <v>4</v>
@@ -5028,7 +5049,7 @@
         <v>21</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G11" s="6">
         <v>1</v>
@@ -5037,7 +5058,7 @@
         <v>1.1</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K11" s="6">
         <v>0</v>
@@ -5054,7 +5075,7 @@
         <v>21</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G12" s="6">
         <v>0</v>
@@ -5063,7 +5084,7 @@
         <v>0.8125</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K12" s="6">
         <v>0</v>
@@ -5080,7 +5101,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G13" s="6">
         <v>0</v>
@@ -5089,7 +5110,7 @@
         <v>0.525</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K13" s="6">
         <v>0</v>
@@ -5248,9 +5269,9 @@
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="M1:O1"/>
   </mergeCells>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"0,1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>"普通,南瓜,冰道,炮"</formula1>
@@ -5260,6 +5281,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
       <formula1>"随机,最快,最慢"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
       <formula1>"曾,喷"</formula1>

</xml_diff>